<commit_message>
fixed this error type 2 bug
</commit_message>
<xml_diff>
--- a/excel/Hagen_Prime.xlsx
+++ b/excel/Hagen_Prime.xlsx
@@ -1083,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>

</xml_diff>